<commit_message>
Update BOM after ordering heater and project box
</commit_message>
<xml_diff>
--- a/Circuit Design Files/BOM.xlsx
+++ b/Circuit Design Files/BOM.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
-  <workbookPr filterPrivacy="1"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17760" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="100">
   <si>
     <t>Item Description</t>
   </si>
@@ -75,27 +75,6 @@
     <t>B00650P2ZC</t>
   </si>
   <si>
-    <t>Plastic Box</t>
-  </si>
-  <si>
-    <t>BiGDUG</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/Plastic-Storage-Containers-School-Solutions/dp/B01DPN1L74/ref=sr_1_30?ie=UTF8&amp;qid=1516787783&amp;sr=8-30&amp;keywords=plastic%20box%20clear%2050l</t>
-  </si>
-  <si>
-    <t>B01DPN1L74</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/Adhere-Fly-Aluminum-Thermostat-Temperature/dp/B01N0Q9RQ4/ref=pd_day0_107_9?_encoding=UTF8&amp;psc=1&amp;refRID=QCTZEQQF5RFKNGRZ3H98</t>
-  </si>
-  <si>
-    <t>B01N0Q9RQ4</t>
-  </si>
-  <si>
-    <t>Adhere To Fly</t>
-  </si>
-  <si>
     <t>Molex</t>
   </si>
   <si>
@@ -297,42 +276,58 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Black Elastic 25 mm</t>
-  </si>
-  <si>
-    <t>12 V 150 W Heater </t>
-  </si>
-  <si>
-    <t>Cut &amp; Sew Cmp.</t>
-  </si>
-  <si>
-    <t>B00U8THDR6</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/Elastic-Smooth-Durable-Quality-Metres/dp/B00U8THDR6/ref=sr_1_2?s=kitchen&amp;ie=UTF8&amp;qid=1517998504&amp;sr=1-2&amp;keywords=black+elastic+25mm</t>
-  </si>
-  <si>
-    <t>Junc. Box 230x150x85</t>
-  </si>
-  <si>
-    <t>Sodial</t>
-  </si>
-  <si>
-    <t>8Z-FIJA-2PSW</t>
-  </si>
-  <si>
-    <t>B00HG7FM26</t>
-  </si>
-  <si>
-    <t>https://www.amazon.co.uk/230mmx150mmx85mm-Waterproof-Plastic-Enclosure-Junction/dp/B00HG7FM26/ref=sr_1_2?ie=UTF8&amp;qid=1517998690&amp;sr=8-2&amp;keywords=230mm+electronic+box</t>
+    <t>Tesco</t>
+  </si>
+  <si>
+    <t>Elastic</t>
+  </si>
+  <si>
+    <t>45 Litre Plastic Box</t>
+  </si>
+  <si>
+    <t>Wham</t>
+  </si>
+  <si>
+    <t>ABS Enclosure</t>
+  </si>
+  <si>
+    <t>Hammond</t>
+  </si>
+  <si>
+    <t>1554SGY</t>
+  </si>
+  <si>
+    <t>818-0457 </t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/general-purpose-enclosures/8180457/</t>
+  </si>
+  <si>
+    <t>50W Heating Element</t>
+  </si>
+  <si>
+    <t>DBK Enclosures</t>
+  </si>
+  <si>
+    <t>HPG-1.5/11-40X35-12-30</t>
+  </si>
+  <si>
+    <t>725-6480 </t>
+  </si>
+  <si>
+    <t>https://uk.rs-online.com/web/p/enclosure-heating-elements/7256480/</t>
+  </si>
+  <si>
+    <t>Total Orders:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;£&quot;#,##0.00;[Red]\-&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="169" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -410,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -442,6 +437,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -731,15 +729,15 @@
   <dimension ref="A1:I216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="164.85546875" bestFit="1" customWidth="1"/>
@@ -750,22 +748,29 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>90</v>
+        <v>83</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F2" s="21">
+        <f>10.66+17.49+7.69+42.25</f>
+        <v>78.09</v>
       </c>
       <c r="I2" s="2"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" s="20" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="I3" s="2"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C4" s="6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -776,13 +781,13 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="D6" s="17" t="s">
         <v>0</v>
@@ -814,7 +819,7 @@
         <v>17.489999999999998</v>
       </c>
       <c r="C8" s="7">
-        <f>A8*B8</f>
+        <f t="shared" ref="C8:C27" si="0">A8*B8</f>
         <v>17.489999999999998</v>
       </c>
       <c r="D8" s="8" t="s">
@@ -844,7 +849,7 @@
         <v>3.98</v>
       </c>
       <c r="C9" s="7">
-        <f>A9*B9</f>
+        <f t="shared" si="0"/>
         <v>7.96</v>
       </c>
       <c r="D9" s="8" t="s">
@@ -867,243 +872,237 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
+      <c r="A10" s="11">
         <v>1</v>
       </c>
       <c r="B10" s="7">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C10" s="7">
-        <f>A10*B10</f>
-        <v>11</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="F10" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="G10" s="8" t="s">
-        <v>6</v>
-      </c>
       <c r="H10" s="9" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>20</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
+      <c r="A11" s="11">
         <v>1</v>
       </c>
-      <c r="B11" s="7">
-        <v>1.71</v>
-      </c>
+      <c r="B11" s="7"/>
       <c r="C11" s="7">
-        <f>A11*B11</f>
-        <v>1.71</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D11" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="20">
+        <v>1</v>
+      </c>
+      <c r="B12" s="7">
+        <v>21.49</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>21.49</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="I12" s="10" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
+        <v>2</v>
+      </c>
+      <c r="B13" s="7">
+        <v>10.38</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="0"/>
+        <v>20.76</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H11" s="9" t="s">
+      <c r="E13" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6">
-        <v>1</v>
-      </c>
-      <c r="B12" s="7">
-        <v>6.14</v>
-      </c>
-      <c r="C12" s="7">
-        <f>A12*B12</f>
-        <v>6.14</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="6">
-        <v>1</v>
-      </c>
-      <c r="B13" s="7">
-        <v>7.95</v>
-      </c>
-      <c r="C13" s="7">
-        <f>A13*B13</f>
-        <v>7.95</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="G13" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="I13" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>101</v>
-      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="20">
+      <c r="A14" s="11">
         <v>2</v>
       </c>
       <c r="B14" s="7">
         <v>0.36</v>
       </c>
       <c r="C14" s="7">
-        <f>A14*B14</f>
+        <f t="shared" si="0"/>
         <v>0.72</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="20">
+      <c r="A15" s="11">
         <v>2</v>
       </c>
       <c r="B15" s="7">
         <v>0.2</v>
       </c>
       <c r="C15" s="7">
-        <f>A15*B15</f>
+        <f t="shared" si="0"/>
         <v>0.4</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>32</v>
-      </c>
       <c r="G15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="H15" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>33</v>
-      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="20">
+      <c r="A16" s="11">
         <v>4</v>
       </c>
       <c r="B16" s="7">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="C16" s="7">
-        <f>A16*B16</f>
+        <f t="shared" si="0"/>
         <v>0.28000000000000003</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I16" s="10" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+      <c r="A17" s="11">
         <v>1</v>
       </c>
       <c r="B17" s="7">
         <v>0.3</v>
       </c>
       <c r="C17" s="7">
-        <f>A17*B17</f>
+        <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F17" s="13">
         <v>470531000</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="I17" s="10" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1114,26 +1113,26 @@
         <v>0.11</v>
       </c>
       <c r="C18" s="7">
-        <f>A18*B18</f>
+        <f t="shared" si="0"/>
         <v>1.65</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1144,26 +1143,26 @@
         <v>0.16</v>
       </c>
       <c r="C19" s="7">
-        <f>A19*B19</f>
+        <f t="shared" si="0"/>
         <v>0.32</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F19" s="15">
         <v>22232031</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="I19" s="10" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1174,116 +1173,116 @@
         <v>0.12</v>
       </c>
       <c r="C20" s="7">
-        <f>A20*B20</f>
+        <f t="shared" si="0"/>
         <v>0.24</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F20" s="13">
         <v>22012037</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H20" s="9" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="I20" s="10" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="20">
+      <c r="A21" s="11">
         <v>1</v>
       </c>
       <c r="B21" s="7">
         <v>0.54</v>
       </c>
       <c r="C21" s="7">
-        <f>A21*B21</f>
+        <f t="shared" si="0"/>
         <v>0.54</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F21" s="13">
         <v>39281043</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="20">
+      <c r="A22" s="11">
         <v>1</v>
       </c>
       <c r="B22" s="7">
         <v>0.37</v>
       </c>
       <c r="C22" s="7">
-        <f>A22*B22</f>
+        <f t="shared" si="0"/>
         <v>0.37</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="20">
+      <c r="A23" s="11">
         <v>1</v>
       </c>
       <c r="B23" s="7">
         <v>0.42</v>
       </c>
       <c r="C23" s="7">
-        <f>A23*B23</f>
+        <f t="shared" si="0"/>
         <v>0.42</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1294,26 +1293,26 @@
         <v>0.11</v>
       </c>
       <c r="C24" s="7">
-        <f>A24*B24</f>
+        <f t="shared" si="0"/>
         <v>0.22</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -1324,86 +1323,86 @@
         <v>0.09</v>
       </c>
       <c r="C25" s="7">
-        <f>A25*B25</f>
+        <f t="shared" si="0"/>
         <v>0.18</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="F25" s="16" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="I25" s="10" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="20">
+      <c r="A26" s="11">
         <v>2</v>
       </c>
       <c r="B26" s="7">
         <v>0.34</v>
       </c>
       <c r="C26" s="7">
-        <f>A26*B26</f>
+        <f t="shared" si="0"/>
         <v>0.68</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="F26" s="16" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H26" s="9" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I26" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="20">
+      <c r="A27" s="11">
         <v>2</v>
       </c>
       <c r="B27" s="7">
         <v>1.17</v>
       </c>
       <c r="C27" s="7">
-        <f>A27*B27</f>
+        <f t="shared" si="0"/>
         <v>2.34</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="F27" s="16" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="I27" s="10" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -1413,11 +1412,11 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="C29" s="7">
         <f>SUM(C8:C27)</f>
-        <v>60.91</v>
+        <v>83.360000000000028</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="2"/>

</xml_diff>